<commit_message>
update to supply chain indicator scores
</commit_message>
<xml_diff>
--- a/dmsan/comparison/scores/other_indicator_scores.xlsx
+++ b/dmsan/comparison/scores/other_indicator_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\gates\scores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\comparison\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B936F01-7091-4071-B6B2-771E46C51E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A469F-F4E2-4035-9545-3C68D5F3F41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10380" firstSheet="8" activeTab="11" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSummary" sheetId="25" r:id="rId1"/>
@@ -2299,8 +2299,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2363,7 +2363,9 @@
       <c r="F2" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="20">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>16</v>
       </c>
@@ -2387,7 +2389,9 @@
       <c r="F3" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
       <c r="J3" t="s">
         <v>16</v>
       </c>
@@ -2525,8 +2529,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2587,7 +2591,7 @@
         <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -2613,7 +2617,7 @@
         <v>148</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -2639,10 +2643,10 @@
         <v>149</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -2665,10 +2669,10 @@
         <v>234</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -2691,10 +2695,10 @@
         <v>235</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -2717,10 +2721,10 @@
         <v>236</v>
       </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -3580,7 +3584,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3783,7 +3787,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3993,7 +3997,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4418,7 +4422,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4630,7 +4634,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>